<commit_message>
swapped err7127606 and 607
</commit_message>
<xml_diff>
--- a/pema_overview_COI_batch1.xlsx
+++ b/pema_overview_COI_batch1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katrinae\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katrinae\Desktop\GitHub\analysis_release_001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{194122EB-2F4F-48C9-B41B-77704820D7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E210715-D2EA-4EA5-97FC-C45B073D45A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="13800" windowHeight="8580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="1440" windowWidth="16270" windowHeight="9290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COI" sheetId="3" r:id="rId1"/>
@@ -2506,9 +2506,6 @@
     <t>ARMS-COI-Laesoe2-190819-200811-MF500-A_S183_L001_R2_001.fastq.gz</t>
   </si>
   <si>
-    <t>ERR7127606</t>
-  </si>
-  <si>
     <t>ARMS-COI-BelgianCoast-ZBE1-190924-200303-MT100_S199_L001_R1_001.fastq.gz</t>
   </si>
   <si>
@@ -2681,6 +2678,9 @@
   </si>
   <si>
     <t>ERR9632101</t>
+  </si>
+  <si>
+    <t>ERR7127607</t>
   </si>
 </sst>
 </file>
@@ -2797,23 +2797,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3036,8 +3036,8 @@
   </sheetPr>
   <dimension ref="A1:T191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="R100" workbookViewId="0">
+      <selection activeCell="S107" sqref="S107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3114,7 +3114,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="20" t="s">
         <v>308</v>
       </c>
       <c r="B2" s="3">
@@ -3171,7 +3171,7 @@
       <c r="S2" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="T2" s="26" t="s">
+      <c r="T2" s="20" t="s">
         <v>315</v>
       </c>
     </row>
@@ -4470,7 +4470,7 @@
       <c r="T25" s="21"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="22" t="s">
         <v>373</v>
       </c>
       <c r="B26" s="9">
@@ -4527,7 +4527,7 @@
       <c r="S26" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="T26" s="24" t="s">
+      <c r="T26" s="22" t="s">
         <v>379</v>
       </c>
     </row>
@@ -6794,7 +6794,7 @@
       <c r="T65" s="21"/>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A66" s="25" t="s">
+      <c r="A66" s="23" t="s">
         <v>497</v>
       </c>
       <c r="B66" s="11">
@@ -6851,7 +6851,7 @@
       <c r="S66" s="8" t="s">
         <v>502</v>
       </c>
-      <c r="T66" s="25" t="s">
+      <c r="T66" s="23" t="s">
         <v>503</v>
       </c>
     </row>
@@ -7378,7 +7378,7 @@
       <c r="T75" s="21"/>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A76" s="20" t="s">
+      <c r="A76" s="24" t="s">
         <v>531</v>
       </c>
       <c r="B76" s="13">
@@ -7435,7 +7435,7 @@
       <c r="S76" s="8" t="s">
         <v>536</v>
       </c>
-      <c r="T76" s="20" t="s">
+      <c r="T76" s="24" t="s">
         <v>537</v>
       </c>
     </row>
@@ -9524,7 +9524,7 @@
       <c r="T112" s="21"/>
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A113" s="22" t="s">
+      <c r="A113" s="25" t="s">
         <v>643</v>
       </c>
       <c r="B113" s="15">
@@ -9581,7 +9581,7 @@
       <c r="S113" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="T113" s="22" t="s">
+      <c r="T113" s="25" t="s">
         <v>649</v>
       </c>
     </row>
@@ -13061,7 +13061,7 @@
         <v>313</v>
       </c>
       <c r="S173" s="17" t="s">
-        <v>828</v>
+        <v>886</v>
       </c>
       <c r="T173" s="21"/>
     </row>
@@ -13077,10 +13077,10 @@
         <v>645</v>
       </c>
       <c r="E174" s="16" t="s">
+        <v>828</v>
+      </c>
+      <c r="F174" s="16" t="s">
         <v>829</v>
-      </c>
-      <c r="F174" s="16" t="s">
-        <v>830</v>
       </c>
       <c r="G174" s="16" t="s">
         <v>20</v>
@@ -13119,28 +13119,28 @@
         <v>313</v>
       </c>
       <c r="S174" s="17" t="s">
+        <v>830</v>
+      </c>
+      <c r="T174" s="21"/>
+    </row>
+    <row r="175" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A175" s="26" t="s">
         <v>831</v>
-      </c>
-      <c r="T174" s="21"/>
-    </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A175" s="23" t="s">
-        <v>832</v>
       </c>
       <c r="B175" s="18">
         <v>44562</v>
       </c>
       <c r="C175" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D175" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D175" s="6" t="s">
+      <c r="E175" s="6" t="s">
         <v>834</v>
       </c>
-      <c r="E175" s="6" t="s">
+      <c r="F175" s="6" t="s">
         <v>835</v>
-      </c>
-      <c r="F175" s="6" t="s">
-        <v>836</v>
       </c>
       <c r="G175" s="19" t="s">
         <v>20</v>
@@ -13179,10 +13179,10 @@
         <v>313</v>
       </c>
       <c r="S175" s="8" t="s">
+        <v>836</v>
+      </c>
+      <c r="T175" s="26" t="s">
         <v>837</v>
-      </c>
-      <c r="T175" s="23" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="176" spans="1:20" x14ac:dyDescent="0.3">
@@ -13191,16 +13191,16 @@
         <v>44562</v>
       </c>
       <c r="C176" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D176" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D176" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E176" s="6" t="s">
+        <v>838</v>
+      </c>
+      <c r="F176" s="6" t="s">
         <v>839</v>
-      </c>
-      <c r="F176" s="6" t="s">
-        <v>840</v>
       </c>
       <c r="G176" s="19" t="s">
         <v>20</v>
@@ -13239,7 +13239,7 @@
         <v>313</v>
       </c>
       <c r="S176" s="8" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="T176" s="21"/>
     </row>
@@ -13249,16 +13249,16 @@
         <v>44562</v>
       </c>
       <c r="C177" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D177" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D177" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E177" s="6" t="s">
+        <v>841</v>
+      </c>
+      <c r="F177" s="6" t="s">
         <v>842</v>
-      </c>
-      <c r="F177" s="6" t="s">
-        <v>843</v>
       </c>
       <c r="G177" s="19" t="s">
         <v>20</v>
@@ -13297,7 +13297,7 @@
         <v>313</v>
       </c>
       <c r="S177" s="8" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="T177" s="21"/>
     </row>
@@ -13307,16 +13307,16 @@
         <v>44562</v>
       </c>
       <c r="C178" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D178" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D178" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E178" s="6" t="s">
+        <v>844</v>
+      </c>
+      <c r="F178" s="6" t="s">
         <v>845</v>
-      </c>
-      <c r="F178" s="6" t="s">
-        <v>846</v>
       </c>
       <c r="G178" s="19" t="s">
         <v>20</v>
@@ -13355,7 +13355,7 @@
         <v>313</v>
       </c>
       <c r="S178" s="8" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="T178" s="21"/>
     </row>
@@ -13365,16 +13365,16 @@
         <v>44562</v>
       </c>
       <c r="C179" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D179" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D179" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E179" s="6" t="s">
+        <v>847</v>
+      </c>
+      <c r="F179" s="6" t="s">
         <v>848</v>
-      </c>
-      <c r="F179" s="6" t="s">
-        <v>849</v>
       </c>
       <c r="G179" s="19" t="s">
         <v>20</v>
@@ -13413,7 +13413,7 @@
         <v>313</v>
       </c>
       <c r="S179" s="8" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="T179" s="21"/>
     </row>
@@ -13423,16 +13423,16 @@
         <v>44562</v>
       </c>
       <c r="C180" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D180" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D180" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E180" s="6" t="s">
+        <v>850</v>
+      </c>
+      <c r="F180" s="6" t="s">
         <v>851</v>
-      </c>
-      <c r="F180" s="6" t="s">
-        <v>852</v>
       </c>
       <c r="G180" s="19" t="s">
         <v>20</v>
@@ -13471,7 +13471,7 @@
         <v>313</v>
       </c>
       <c r="S180" s="8" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="T180" s="21"/>
     </row>
@@ -13481,16 +13481,16 @@
         <v>44562</v>
       </c>
       <c r="C181" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D181" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D181" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E181" s="6" t="s">
+        <v>853</v>
+      </c>
+      <c r="F181" s="6" t="s">
         <v>854</v>
-      </c>
-      <c r="F181" s="6" t="s">
-        <v>855</v>
       </c>
       <c r="G181" s="19" t="s">
         <v>20</v>
@@ -13529,7 +13529,7 @@
         <v>313</v>
       </c>
       <c r="S181" s="8" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="T181" s="21"/>
     </row>
@@ -13539,16 +13539,16 @@
         <v>44562</v>
       </c>
       <c r="C182" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D182" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D182" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E182" s="6" t="s">
+        <v>856</v>
+      </c>
+      <c r="F182" s="6" t="s">
         <v>857</v>
-      </c>
-      <c r="F182" s="6" t="s">
-        <v>858</v>
       </c>
       <c r="G182" s="19" t="s">
         <v>20</v>
@@ -13587,7 +13587,7 @@
         <v>313</v>
       </c>
       <c r="S182" s="8" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="T182" s="21"/>
     </row>
@@ -13597,16 +13597,16 @@
         <v>44562</v>
       </c>
       <c r="C183" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D183" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D183" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E183" s="6" t="s">
+        <v>859</v>
+      </c>
+      <c r="F183" s="6" t="s">
         <v>860</v>
-      </c>
-      <c r="F183" s="6" t="s">
-        <v>861</v>
       </c>
       <c r="G183" s="19" t="s">
         <v>20</v>
@@ -13645,7 +13645,7 @@
         <v>313</v>
       </c>
       <c r="S183" s="8" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="T183" s="21"/>
     </row>
@@ -13655,16 +13655,16 @@
         <v>44562</v>
       </c>
       <c r="C184" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D184" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D184" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E184" s="6" t="s">
+        <v>862</v>
+      </c>
+      <c r="F184" s="6" t="s">
         <v>863</v>
-      </c>
-      <c r="F184" s="6" t="s">
-        <v>864</v>
       </c>
       <c r="G184" s="19" t="s">
         <v>20</v>
@@ -13703,7 +13703,7 @@
         <v>313</v>
       </c>
       <c r="S184" s="8" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="T184" s="21"/>
     </row>
@@ -13713,16 +13713,16 @@
         <v>44562</v>
       </c>
       <c r="C185" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D185" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D185" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E185" s="6" t="s">
+        <v>865</v>
+      </c>
+      <c r="F185" s="6" t="s">
         <v>866</v>
-      </c>
-      <c r="F185" s="6" t="s">
-        <v>867</v>
       </c>
       <c r="G185" s="19" t="s">
         <v>20</v>
@@ -13761,7 +13761,7 @@
         <v>313</v>
       </c>
       <c r="S185" s="8" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="T185" s="21"/>
     </row>
@@ -13771,16 +13771,16 @@
         <v>44562</v>
       </c>
       <c r="C186" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D186" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D186" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E186" s="6" t="s">
+        <v>868</v>
+      </c>
+      <c r="F186" s="6" t="s">
         <v>869</v>
-      </c>
-      <c r="F186" s="6" t="s">
-        <v>870</v>
       </c>
       <c r="G186" s="19" t="s">
         <v>20</v>
@@ -13819,7 +13819,7 @@
         <v>313</v>
       </c>
       <c r="S186" s="6" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="T186" s="21"/>
     </row>
@@ -13829,16 +13829,16 @@
         <v>44562</v>
       </c>
       <c r="C187" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D187" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D187" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E187" s="6" t="s">
+        <v>871</v>
+      </c>
+      <c r="F187" s="6" t="s">
         <v>872</v>
-      </c>
-      <c r="F187" s="6" t="s">
-        <v>873</v>
       </c>
       <c r="G187" s="19" t="s">
         <v>20</v>
@@ -13877,7 +13877,7 @@
         <v>313</v>
       </c>
       <c r="S187" s="6" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="T187" s="21"/>
     </row>
@@ -13887,16 +13887,16 @@
         <v>44562</v>
       </c>
       <c r="C188" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D188" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D188" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E188" s="6" t="s">
+        <v>874</v>
+      </c>
+      <c r="F188" s="6" t="s">
         <v>875</v>
-      </c>
-      <c r="F188" s="6" t="s">
-        <v>876</v>
       </c>
       <c r="G188" s="19" t="s">
         <v>20</v>
@@ -13935,7 +13935,7 @@
         <v>313</v>
       </c>
       <c r="S188" s="6" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="T188" s="21"/>
     </row>
@@ -13945,16 +13945,16 @@
         <v>44562</v>
       </c>
       <c r="C189" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D189" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D189" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E189" s="6" t="s">
+        <v>877</v>
+      </c>
+      <c r="F189" s="6" t="s">
         <v>878</v>
-      </c>
-      <c r="F189" s="6" t="s">
-        <v>879</v>
       </c>
       <c r="G189" s="19" t="s">
         <v>20</v>
@@ -13993,7 +13993,7 @@
         <v>313</v>
       </c>
       <c r="S189" s="6" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="T189" s="21"/>
     </row>
@@ -14003,16 +14003,16 @@
         <v>44562</v>
       </c>
       <c r="C190" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D190" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D190" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E190" s="6" t="s">
+        <v>880</v>
+      </c>
+      <c r="F190" s="6" t="s">
         <v>881</v>
-      </c>
-      <c r="F190" s="6" t="s">
-        <v>882</v>
       </c>
       <c r="G190" s="19" t="s">
         <v>20</v>
@@ -14051,7 +14051,7 @@
         <v>313</v>
       </c>
       <c r="S190" s="6" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="T190" s="21"/>
     </row>
@@ -14061,16 +14061,16 @@
         <v>44562</v>
       </c>
       <c r="C191" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="D191" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="D191" s="6" t="s">
-        <v>834</v>
-      </c>
       <c r="E191" s="6" t="s">
+        <v>883</v>
+      </c>
+      <c r="F191" s="6" t="s">
         <v>884</v>
-      </c>
-      <c r="F191" s="6" t="s">
-        <v>885</v>
       </c>
       <c r="G191" s="19" t="s">
         <v>20</v>
@@ -14109,24 +14109,24 @@
         <v>313</v>
       </c>
       <c r="S191" s="6" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="T191" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A76:A112"/>
+    <mergeCell ref="A113:A174"/>
+    <mergeCell ref="A175:A191"/>
+    <mergeCell ref="T113:T174"/>
+    <mergeCell ref="T175:T191"/>
+    <mergeCell ref="T76:T112"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="T2:T25"/>
     <mergeCell ref="A26:A65"/>
     <mergeCell ref="T26:T65"/>
     <mergeCell ref="A66:A75"/>
     <mergeCell ref="T66:T75"/>
-    <mergeCell ref="A76:A112"/>
-    <mergeCell ref="A113:A174"/>
-    <mergeCell ref="A175:A191"/>
-    <mergeCell ref="T113:T174"/>
-    <mergeCell ref="T175:T191"/>
-    <mergeCell ref="T76:T112"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>